<commit_message>
update entregable 1 y 2
</commit_message>
<xml_diff>
--- a/src/Excel/entregable1/AltaCuentaCTS.xlsx
+++ b/src/Excel/entregable1/AltaCuentaCTS.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Proyectos\Regresion\src\Excel\entregable1\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7A52E665-F158-444C-B237-1E4901568462}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7350214B-8828-4AE9-BBFE-599EE6C70773}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -42,9 +42,6 @@
     <t>ruc</t>
   </si>
   <si>
-    <t>razon</t>
-  </si>
-  <si>
     <t>SCISNEROSA1</t>
   </si>
   <si>
@@ -91,6 +88,9 @@
   </si>
   <si>
     <t>CodCliente</t>
+  </si>
+  <si>
+    <t>motivoApertura</t>
   </si>
 </sst>
 </file>
@@ -448,7 +448,7 @@
   <dimension ref="A1:K2"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.7265625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -458,7 +458,7 @@
     <col min="3" max="3" width="10.36328125" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="5" max="5" width="15.1796875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="6" max="6" width="9.54296875" bestFit="1" customWidth="1" collapsed="1"/>
-    <col min="7" max="7" width="12.54296875" bestFit="1" customWidth="1" collapsed="1"/>
+    <col min="7" max="7" width="14.08984375" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="9" max="9" width="23.54296875" customWidth="1" collapsed="1"/>
     <col min="10" max="10" width="19.54296875" bestFit="1" customWidth="1" collapsed="1"/>
     <col min="11" max="11" width="11.6328125" bestFit="1" customWidth="1" collapsed="1"/>
@@ -472,7 +472,7 @@
         <v>1</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D1" s="2" t="s">
         <v>2</v>
@@ -484,54 +484,54 @@
         <v>4</v>
       </c>
       <c r="G1" s="2" t="s">
-        <v>5</v>
+        <v>21</v>
       </c>
       <c r="H1" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="I1" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="3" t="s">
+      <c r="J1" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="3" t="s">
-        <v>14</v>
-      </c>
       <c r="K1" s="3" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
     </row>
     <row r="2" spans="1:11" x14ac:dyDescent="0.35">
       <c r="A2" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="C2" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="D2" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="1" t="s">
+      <c r="E2" t="s">
         <v>9</v>
       </c>
-      <c r="E2" t="s">
+      <c r="F2" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="F2" s="1" t="s">
-        <v>11</v>
-      </c>
       <c r="G2" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="H2" t="s">
+        <v>16</v>
+      </c>
+      <c r="I2" t="s">
+        <v>18</v>
+      </c>
+      <c r="J2" t="s">
+        <v>19</v>
+      </c>
+      <c r="K2" t="s">
         <v>17</v>
-      </c>
-      <c r="I2" t="s">
-        <v>19</v>
-      </c>
-      <c r="J2" t="s">
-        <v>20</v>
-      </c>
-      <c r="K2" t="s">
-        <v>18</v>
       </c>
     </row>
   </sheetData>

</xml_diff>